<commit_message>
Used the cumrisk function to calculate AJ estimates - faster. Further, incroporated treatment effect heterogeneity on the ratio scale in the Excel files.
</commit_message>
<xml_diff>
--- a/Parameters_Abortion15_Preeclampsia07.xlsx
+++ b/Parameters_Abortion15_Preeclampsia07.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaselatour/preg_cohort_construction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8940622-C7C2-284B-8621-AAECE448701C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15A28F7-B3AD-2D4E-9D07-5C970468AB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30080" yWindow="-700" windowWidth="28800" windowHeight="16260" activeTab="2" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{EDFB6D7C-8216-ED43-8AA6-178B9CD2875A}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="13" r:id="rId1"/>
@@ -1989,10 +1989,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBAD042-1D8C-E044-AB59-2B80CE0D260D}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2000,13 +2000,13 @@
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="16"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2030,13 +2030,13 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="16"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2052,29 +2052,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="8">
+        <v>2</v>
+      </c>
+      <c r="C9">
         <v>1.25</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="8">
+        <v>3</v>
+      </c>
+      <c r="C10">
         <v>1.5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="16"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2082,7 +2088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2090,7 +2096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2098,7 +2104,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2140,7 +2146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0633E7-A8AC-2448-856C-6ACF1A963AAB}">
   <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3057,7 +3063,7 @@
       </c>
       <c r="C50" s="3">
         <f>C9*SimParameters!B9</f>
-        <v>0.11249999999999999</v>
+        <v>0.18</v>
       </c>
       <c r="D50" s="3">
         <f t="shared" si="1"/>
@@ -3065,7 +3071,7 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="2"/>
-        <v>0.88749999999999996</v>
+        <v>0.82000000000000006</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -3077,7 +3083,7 @@
       </c>
       <c r="C51" s="3">
         <f>C10*SimParameters!B9</f>
-        <v>1.8749999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D51" s="3">
         <f t="shared" si="1"/>
@@ -3085,7 +3091,7 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="2"/>
-        <v>0.98124999999999996</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -3097,7 +3103,7 @@
       </c>
       <c r="C52" s="3">
         <f>C11*SimParameters!B9</f>
-        <v>1.8749999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D52" s="3">
         <f t="shared" si="1"/>
@@ -3105,7 +3111,7 @@
       </c>
       <c r="E52" s="3">
         <f t="shared" si="2"/>
-        <v>0.98124999999999996</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -3117,7 +3123,7 @@
       </c>
       <c r="C53" s="3">
         <f>C12*SimParameters!B9</f>
-        <v>1.8749999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D53" s="3">
         <f t="shared" si="1"/>
@@ -3125,7 +3131,7 @@
       </c>
       <c r="E53" s="3">
         <f t="shared" si="2"/>
-        <v>0.98124999999999996</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -3137,7 +3143,7 @@
       </c>
       <c r="C54" s="3">
         <f>C13*SimParameters!B9</f>
-        <v>1.8749999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D54" s="3">
         <f t="shared" si="1"/>
@@ -3145,7 +3151,7 @@
       </c>
       <c r="E54" s="3">
         <f t="shared" si="2"/>
-        <v>0.98124999999999996</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -3157,7 +3163,7 @@
       </c>
       <c r="C55" s="3">
         <f>C14*SimParameters!B9</f>
-        <v>1.2500000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D55" s="3">
         <f t="shared" si="1"/>
@@ -3165,7 +3171,7 @@
       </c>
       <c r="E55" s="3">
         <f t="shared" si="2"/>
-        <v>0.98750000000000004</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -3177,7 +3183,7 @@
       </c>
       <c r="C56" s="3">
         <f>C15*SimParameters!B9</f>
-        <v>1.2500000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D56" s="3">
         <f t="shared" si="1"/>
@@ -3185,7 +3191,7 @@
       </c>
       <c r="E56" s="3">
         <f t="shared" si="2"/>
-        <v>0.98750000000000004</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -3197,7 +3203,7 @@
       </c>
       <c r="C57" s="3">
         <f>C16*SimParameters!B9</f>
-        <v>1.2500000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D57" s="3">
         <f t="shared" si="1"/>
@@ -3205,7 +3211,7 @@
       </c>
       <c r="E57" s="3">
         <f t="shared" si="2"/>
-        <v>0.98750000000000004</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -3217,7 +3223,7 @@
       </c>
       <c r="C58" s="3">
         <f>C17*SimParameters!B9</f>
-        <v>1.2500000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D58" s="3">
         <f t="shared" si="1"/>
@@ -3225,7 +3231,7 @@
       </c>
       <c r="E58" s="3">
         <f t="shared" si="2"/>
-        <v>0.98750000000000004</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -3237,7 +3243,7 @@
       </c>
       <c r="C59" s="3">
         <f>C18*SimParameters!B9</f>
-        <v>1E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="D59" s="3">
         <f t="shared" si="1"/>
@@ -3245,7 +3251,7 @@
       </c>
       <c r="E59" s="3">
         <f t="shared" si="2"/>
-        <v>0.999</v>
+        <v>0.99839999999999995</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -3876,7 +3882,7 @@
       </c>
       <c r="C91" s="4">
         <f>C9*SimParameters!B10</f>
-        <v>0.13500000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="D91" s="4">
         <f t="shared" si="4"/>
@@ -3884,7 +3890,7 @@
       </c>
       <c r="E91" s="4">
         <f t="shared" si="5"/>
-        <v>0.86499999999999999</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -3896,7 +3902,7 @@
       </c>
       <c r="C92" s="4">
         <f>C10*SimParameters!B10</f>
-        <v>2.2499999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D92" s="4">
         <f t="shared" si="4"/>
@@ -3904,7 +3910,7 @@
       </c>
       <c r="E92" s="4">
         <f t="shared" si="5"/>
-        <v>0.97750000000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -3916,7 +3922,7 @@
       </c>
       <c r="C93" s="4">
         <f>C11*SimParameters!B10</f>
-        <v>2.2499999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D93" s="4">
         <f t="shared" si="4"/>
@@ -3924,7 +3930,7 @@
       </c>
       <c r="E93" s="4">
         <f t="shared" si="5"/>
-        <v>0.97750000000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -3936,7 +3942,7 @@
       </c>
       <c r="C94" s="4">
         <f>C12*SimParameters!B10</f>
-        <v>2.2499999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D94" s="4">
         <f t="shared" si="4"/>
@@ -3944,7 +3950,7 @@
       </c>
       <c r="E94" s="4">
         <f t="shared" si="5"/>
-        <v>0.97750000000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -3956,7 +3962,7 @@
       </c>
       <c r="C95" s="4">
         <f>C13*SimParameters!B10</f>
-        <v>2.2499999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D95" s="4">
         <f t="shared" si="4"/>
@@ -3964,7 +3970,7 @@
       </c>
       <c r="E95" s="4">
         <f t="shared" si="5"/>
-        <v>0.97750000000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -3976,7 +3982,7 @@
       </c>
       <c r="C96" s="4">
         <f>C14*SimParameters!B10</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D96" s="4">
         <f t="shared" si="4"/>
@@ -3984,7 +3990,7 @@
       </c>
       <c r="E96" s="4">
         <f t="shared" si="5"/>
-        <v>0.98499999999999999</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -3996,7 +4002,7 @@
       </c>
       <c r="C97" s="4">
         <f>C15*SimParameters!B10</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D97" s="4">
         <f t="shared" si="4"/>
@@ -4004,7 +4010,7 @@
       </c>
       <c r="E97" s="4">
         <f t="shared" si="5"/>
-        <v>0.98499999999999999</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -4016,7 +4022,7 @@
       </c>
       <c r="C98" s="4">
         <f>C16*SimParameters!B10</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D98" s="4">
         <f t="shared" si="4"/>
@@ -4024,7 +4030,7 @@
       </c>
       <c r="E98" s="4">
         <f t="shared" si="5"/>
-        <v>0.98499999999999999</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -4036,7 +4042,7 @@
       </c>
       <c r="C99" s="4">
         <f>C17*SimParameters!B10</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D99" s="4">
         <f t="shared" si="4"/>
@@ -4044,7 +4050,7 @@
       </c>
       <c r="E99" s="4">
         <f t="shared" si="5"/>
-        <v>0.98499999999999999</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -4056,7 +4062,7 @@
       </c>
       <c r="C100" s="4">
         <f>C18*SimParameters!B10</f>
-        <v>1.2000000000000001E-3</v>
+        <v>2.4000000000000002E-3</v>
       </c>
       <c r="D100" s="4">
         <f t="shared" si="4"/>
@@ -4064,7 +4070,7 @@
       </c>
       <c r="E100" s="4">
         <f t="shared" si="5"/>
-        <v>0.99880000000000002</v>
+        <v>0.99760000000000004</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -5553,7 +5559,7 @@
       </c>
       <c r="C50" s="3">
         <f>potential_preg_untrt!C50*SimParameters!$B$3</f>
-        <v>0.16874999999999998</v>
+        <v>0.27</v>
       </c>
       <c r="D50" s="3">
         <f>potential_preg_untrt!D50</f>
@@ -5561,7 +5567,7 @@
       </c>
       <c r="E50" s="3">
         <f t="shared" si="1"/>
-        <v>0.83125000000000004</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -5573,7 +5579,7 @@
       </c>
       <c r="C51" s="3">
         <f>potential_preg_untrt!C51*SimParameters!$B$3</f>
-        <v>2.8124999999999997E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D51" s="3">
         <f>potential_preg_untrt!D51</f>
@@ -5581,7 +5587,7 @@
       </c>
       <c r="E51" s="3">
         <f t="shared" si="1"/>
-        <v>0.97187500000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -5593,7 +5599,7 @@
       </c>
       <c r="C52" s="3">
         <f>potential_preg_untrt!C52*SimParameters!$B$3</f>
-        <v>2.8124999999999997E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D52" s="3">
         <f>potential_preg_untrt!D52</f>
@@ -5601,7 +5607,7 @@
       </c>
       <c r="E52" s="3">
         <f t="shared" si="1"/>
-        <v>0.97187500000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -5613,7 +5619,7 @@
       </c>
       <c r="C53" s="3">
         <f>potential_preg_untrt!C53*SimParameters!$B$3</f>
-        <v>2.8124999999999997E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D53" s="3">
         <f>potential_preg_untrt!D53</f>
@@ -5621,7 +5627,7 @@
       </c>
       <c r="E53" s="3">
         <f t="shared" si="1"/>
-        <v>0.97187500000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -5633,7 +5639,7 @@
       </c>
       <c r="C54" s="3">
         <f>potential_preg_untrt!C54*SimParameters!$B$3</f>
-        <v>2.8124999999999997E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D54" s="3">
         <f>potential_preg_untrt!D54</f>
@@ -5641,7 +5647,7 @@
       </c>
       <c r="E54" s="3">
         <f t="shared" si="1"/>
-        <v>0.97187500000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -5653,7 +5659,7 @@
       </c>
       <c r="C55" s="3">
         <f>potential_preg_untrt!C55*SimParameters!$B$3</f>
-        <v>1.8750000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D55" s="3">
         <f>potential_preg_untrt!D55</f>
@@ -5661,7 +5667,7 @@
       </c>
       <c r="E55" s="3">
         <f t="shared" si="1"/>
-        <v>0.98124999999999996</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -5673,7 +5679,7 @@
       </c>
       <c r="C56" s="3">
         <f>potential_preg_untrt!C56*SimParameters!$B$3</f>
-        <v>1.8750000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D56" s="3">
         <f>potential_preg_untrt!D56</f>
@@ -5681,7 +5687,7 @@
       </c>
       <c r="E56" s="3">
         <f t="shared" si="1"/>
-        <v>0.98124999999999996</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -5693,7 +5699,7 @@
       </c>
       <c r="C57" s="3">
         <f>potential_preg_untrt!C57*SimParameters!$B$3</f>
-        <v>1.8750000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D57" s="3">
         <f>potential_preg_untrt!D57</f>
@@ -5701,7 +5707,7 @@
       </c>
       <c r="E57" s="3">
         <f t="shared" si="1"/>
-        <v>0.98124999999999996</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -5713,7 +5719,7 @@
       </c>
       <c r="C58" s="3">
         <f>potential_preg_untrt!C58*SimParameters!$B$3</f>
-        <v>1.8750000000000003E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D58" s="3">
         <f>potential_preg_untrt!D58</f>
@@ -5721,7 +5727,7 @@
       </c>
       <c r="E58" s="3">
         <f t="shared" si="1"/>
-        <v>0.98124999999999996</v>
+        <v>0.97</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -5733,7 +5739,7 @@
       </c>
       <c r="C59" s="3">
         <f>potential_preg_untrt!C59*SimParameters!$B$3</f>
-        <v>1.5E-3</v>
+        <v>2.4000000000000002E-3</v>
       </c>
       <c r="D59" s="3">
         <f>potential_preg_untrt!D59</f>
@@ -5741,7 +5747,7 @@
       </c>
       <c r="E59" s="3">
         <f t="shared" si="1"/>
-        <v>0.99850000000000005</v>
+        <v>0.99760000000000004</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -6372,7 +6378,7 @@
       </c>
       <c r="C91" s="4">
         <f>potential_preg_untrt!C91*SimParameters!$B$3</f>
-        <v>0.20250000000000001</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="D91" s="4">
         <f>potential_preg_untrt!D91</f>
@@ -6380,7 +6386,7 @@
       </c>
       <c r="E91" s="4">
         <f t="shared" si="2"/>
-        <v>0.79749999999999999</v>
+        <v>0.59499999999999997</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -6392,7 +6398,7 @@
       </c>
       <c r="C92" s="4">
         <f>potential_preg_untrt!C92*SimParameters!$B$3</f>
-        <v>3.3750000000000002E-2</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="D92" s="4">
         <f>potential_preg_untrt!D92</f>
@@ -6400,7 +6406,7 @@
       </c>
       <c r="E92" s="4">
         <f t="shared" si="2"/>
-        <v>0.96625000000000005</v>
+        <v>0.9325</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -6412,7 +6418,7 @@
       </c>
       <c r="C93" s="4">
         <f>potential_preg_untrt!C93*SimParameters!$B$3</f>
-        <v>3.3750000000000002E-2</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="D93" s="4">
         <f>potential_preg_untrt!D93</f>
@@ -6420,7 +6426,7 @@
       </c>
       <c r="E93" s="4">
         <f t="shared" si="2"/>
-        <v>0.96625000000000005</v>
+        <v>0.9325</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -6432,7 +6438,7 @@
       </c>
       <c r="C94" s="4">
         <f>potential_preg_untrt!C94*SimParameters!$B$3</f>
-        <v>3.3750000000000002E-2</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="D94" s="4">
         <f>potential_preg_untrt!D94</f>
@@ -6440,7 +6446,7 @@
       </c>
       <c r="E94" s="4">
         <f t="shared" si="2"/>
-        <v>0.96625000000000005</v>
+        <v>0.9325</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -6452,7 +6458,7 @@
       </c>
       <c r="C95" s="4">
         <f>potential_preg_untrt!C95*SimParameters!$B$3</f>
-        <v>3.3750000000000002E-2</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="D95" s="4">
         <f>potential_preg_untrt!D95</f>
@@ -6460,7 +6466,7 @@
       </c>
       <c r="E95" s="4">
         <f t="shared" si="2"/>
-        <v>0.96625000000000005</v>
+        <v>0.9325</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -6472,7 +6478,7 @@
       </c>
       <c r="C96" s="4">
         <f>potential_preg_untrt!C96*SimParameters!$B$3</f>
-        <v>2.2499999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D96" s="4">
         <f>potential_preg_untrt!D96</f>
@@ -6480,7 +6486,7 @@
       </c>
       <c r="E96" s="4">
         <f t="shared" si="2"/>
-        <v>0.97750000000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -6492,7 +6498,7 @@
       </c>
       <c r="C97" s="4">
         <f>potential_preg_untrt!C97*SimParameters!$B$3</f>
-        <v>2.2499999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D97" s="4">
         <f>potential_preg_untrt!D97</f>
@@ -6500,7 +6506,7 @@
       </c>
       <c r="E97" s="4">
         <f t="shared" si="2"/>
-        <v>0.97750000000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -6512,7 +6518,7 @@
       </c>
       <c r="C98" s="4">
         <f>potential_preg_untrt!C98*SimParameters!$B$3</f>
-        <v>2.2499999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D98" s="4">
         <f>potential_preg_untrt!D98</f>
@@ -6520,7 +6526,7 @@
       </c>
       <c r="E98" s="4">
         <f t="shared" si="2"/>
-        <v>0.97750000000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -6532,7 +6538,7 @@
       </c>
       <c r="C99" s="4">
         <f>potential_preg_untrt!C99*SimParameters!$B$3</f>
-        <v>2.2499999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D99" s="4">
         <f>potential_preg_untrt!D99</f>
@@ -6540,7 +6546,7 @@
       </c>
       <c r="E99" s="4">
         <f t="shared" si="2"/>
-        <v>0.97750000000000004</v>
+        <v>0.95499999999999996</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -6552,7 +6558,7 @@
       </c>
       <c r="C100" s="4">
         <f>potential_preg_untrt!C100*SimParameters!$B$3</f>
-        <v>1.8000000000000002E-3</v>
+        <v>3.6000000000000003E-3</v>
       </c>
       <c r="D100" s="4">
         <f>potential_preg_untrt!D100</f>
@@ -6560,7 +6566,7 @@
       </c>
       <c r="E100" s="4">
         <f t="shared" si="2"/>
-        <v>0.99819999999999998</v>
+        <v>0.99639999999999995</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -15422,6 +15428,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006F311363ECB49C45BE6A1ABA8AA4E3C9" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bcab42b681813b96043c0b869577973d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7962a6ab-b148-4fb3-9b24-47c6fd02e414" xmlns:ns3="78c38721-2d96-443e-bd32-82c62d4eed8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b36b52368701cf0b88ba8d42da5a3441" ns2:_="" ns3:_="">
     <xsd:import namespace="7962a6ab-b148-4fb3-9b24-47c6fd02e414"/>
@@ -15646,16 +15661,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDB1F164-DDC9-4622-8588-A1C1F4AFED79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15672,12 +15686,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FC4DEEE-E4C1-4BDA-9F3A-10B42714F00A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>